<commit_message>
best third teams code
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/eu/standings_eu_uefa_men.xlsx
+++ b/data/out/wiki/men/uefa/eu/standings_eu_uefa_men.xlsx
@@ -773,7 +773,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Soviet Union']</t>
+          <t>['Soviet Union', 'Netherlands']</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1085,7 +1085,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['Sweden', 'France']</t>
+          <t>['France', 'Sweden']</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2237,7 +2237,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>['Spain', 'Bulgaria']</t>
+          <t>['Bulgaria', 'Spain']</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'France']</t>
+          <t>['France', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>['Spain', 'France']</t>
+          <t>['France', 'Spain']</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -3863,7 +3863,7 @@
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>['Belgium', 'Italy']</t>
+          <t>['Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['Spain', 'Norway']</t>
+          <t>['Norway', 'Spain']</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -4595,7 +4595,7 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>['Netherlands', 'France']</t>
+          <t>['France', 'Netherlands']</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -5015,7 +5015,7 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -5069,7 +5069,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>['Spain', 'Greece']</t>
+          <t>['Greece', 'Spain']</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -5273,7 +5273,7 @@
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -5651,7 +5651,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -5759,7 +5759,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -6437,7 +6437,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -6491,7 +6491,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -6599,7 +6599,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
@@ -7211,7 +7211,7 @@
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr">
         <is>
-          <t>['Romania', 'Netherlands']</t>
+          <t>['Netherlands', 'Romania']</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -7469,7 +7469,7 @@
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -7577,7 +7577,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -7685,7 +7685,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -7781,7 +7781,7 @@
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -7835,7 +7835,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -7889,7 +7889,7 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
@@ -8351,7 +8351,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
@@ -8405,7 +8405,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -8459,7 +8459,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy']</t>
+          <t>['Italy', 'Spain']</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -8501,7 +8501,7 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -8609,7 +8609,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
@@ -8663,7 +8663,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
@@ -8705,7 +8705,7 @@
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="inlineStr">
         <is>
-          <t>['Romania', 'Switzerland', 'France']</t>
+          <t>['France', 'Switzerland', 'Romania']</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -8759,7 +8759,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>['Albania', 'Switzerland', 'France']</t>
+          <t>['France', 'Albania', 'Switzerland']</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
@@ -8801,7 +8801,7 @@
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['England', 'Wales', 'Slovakia']</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -8855,7 +8855,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['England', 'Wales', 'Slovakia']</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
@@ -8909,7 +8909,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['England', 'Wales', 'Slovakia']</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>['Wales', 'Slovakia', 'England']</t>
+          <t>['England', 'Wales', 'Slovakia']</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -9005,7 +9005,7 @@
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr">
         <is>
-          <t>['Germany', 'Northern Ireland', 'Poland']</t>
+          <t>['Northern Ireland', 'Germany', 'Poland']</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -9059,7 +9059,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>['Germany', 'Northern Ireland', 'Poland']</t>
+          <t>['Northern Ireland', 'Germany', 'Poland']</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>['Germany', 'Northern Ireland', 'Poland']</t>
+          <t>['Northern Ireland', 'Germany', 'Poland']</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
@@ -9155,7 +9155,7 @@
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Czech Republic', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>['Spain', 'Czech Republic', 'Croatia']</t>
+          <t>['Czech Republic', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -9317,7 +9317,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -9425,7 +9425,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>['Spain', 'Turkey', 'Croatia']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
@@ -9467,7 +9467,7 @@
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="inlineStr">
         <is>
-          <t>['Belgium', 'Sweden', 'Italy']</t>
+          <t>['Sweden', 'Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Belgium', 'Italy']</t>
+          <t>['Republic of Ireland', 'Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -9575,7 +9575,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Belgium', 'Italy']</t>
+          <t>['Republic of Ireland', 'Italy', 'Belgium']</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -9617,7 +9617,7 @@
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
@@ -9671,7 +9671,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -9725,7 +9725,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
@@ -9779,7 +9779,7 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
@@ -9833,7 +9833,7 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
@@ -9887,7 +9887,7 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
@@ -9941,7 +9941,7 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
@@ -9995,7 +9995,7 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
@@ -10103,7 +10103,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>['Hungary', 'Iceland', 'Portugal']</t>
+          <t>['Portugal', 'Iceland', 'Hungary']</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -10145,7 +10145,7 @@
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -10199,7 +10199,7 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
@@ -10253,7 +10253,7 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -10307,7 +10307,7 @@
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
@@ -10361,7 +10361,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
@@ -10415,7 +10415,7 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>['Wales', 'Switzerland', 'Italy']</t>
+          <t>['Switzerland', 'Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
@@ -10457,7 +10457,7 @@
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Russia', 'Finland', 'Belgium']</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
@@ -10565,7 +10565,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
@@ -10619,7 +10619,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>['Belgium', 'Finland', 'Denmark']</t>
+          <t>['Finland', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
@@ -10673,7 +10673,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Russia', 'Finland', 'Belgium']</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Russia', 'Finland', 'Belgium']</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Russia', 'Finland', 'Belgium']</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -10835,7 +10835,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium', 'Finland']</t>
+          <t>['Russia', 'Finland', 'Belgium']</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -11447,7 +11447,7 @@
       <c r="G212" t="inlineStr"/>
       <c r="H212" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
@@ -11501,7 +11501,7 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I213" t="inlineStr">
@@ -11555,7 +11555,7 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
@@ -11609,7 +11609,7 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I215" t="inlineStr">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
@@ -11717,7 +11717,7 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I217" t="inlineStr">
@@ -11771,7 +11771,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -11825,7 +11825,7 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I219" t="inlineStr">
@@ -11879,7 +11879,7 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I220" t="inlineStr">
@@ -11933,7 +11933,7 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I221" t="inlineStr">
@@ -11987,7 +11987,7 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>['Spain', 'Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Spain', 'Slovakia']</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -12029,7 +12029,7 @@
       <c r="G223" t="inlineStr"/>
       <c r="H223" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany', 'France']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="I223" t="inlineStr">
@@ -12083,7 +12083,7 @@
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['France', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I224" t="inlineStr">
@@ -12137,7 +12137,7 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['France', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
@@ -12191,7 +12191,7 @@
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>['Portugal', 'Hungary', 'France']</t>
+          <t>['France', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
@@ -12245,7 +12245,7 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['France', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I227" t="inlineStr">
@@ -12299,7 +12299,7 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>['Germany', 'France', 'Portugal']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
@@ -12353,7 +12353,7 @@
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Portugal']</t>
+          <t>['France', 'Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I229" t="inlineStr">
@@ -12407,7 +12407,7 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>['Germany', 'France', 'Portugal']</t>
+          <t>['France', 'Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="I230" t="inlineStr">
@@ -12449,7 +12449,7 @@
       <c r="G231" t="inlineStr"/>
       <c r="H231" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="I231" t="inlineStr">
@@ -12503,7 +12503,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Scotland']</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
@@ -12557,7 +12557,7 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>['Germany', 'Scotland', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Scotland']</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
@@ -12611,7 +12611,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>['Hungary', 'Germany', 'Switzerland']</t>
+          <t>['Switzerland', 'Germany', 'Hungary']</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -12653,7 +12653,7 @@
       <c r="G235" t="inlineStr"/>
       <c r="H235" t="inlineStr">
         <is>
-          <t>['Spain', 'Albania', 'Italy']</t>
+          <t>['Italy', 'Albania', 'Spain']</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
@@ -12707,7 +12707,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I236" t="inlineStr">
@@ -12761,7 +12761,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>['Spain', 'Italy', 'Croatia']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>['Spain', 'Croatia', 'Italy']</t>
+          <t>['Italy', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
@@ -12857,7 +12857,7 @@
       <c r="G239" t="inlineStr"/>
       <c r="H239" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="I240" t="inlineStr">
@@ -12965,7 +12965,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="I241" t="inlineStr">
@@ -13019,7 +13019,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -13073,7 +13073,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Denmark', 'Slovenia']</t>
         </is>
       </c>
       <c r="I243" t="inlineStr">
@@ -13115,7 +13115,7 @@
       <c r="G244" t="inlineStr"/>
       <c r="H244" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
@@ -13169,7 +13169,7 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="I245" t="inlineStr">
@@ -13223,7 +13223,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -13277,7 +13277,7 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="I247" t="inlineStr">
@@ -13331,7 +13331,7 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
@@ -13385,7 +13385,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['France', 'Netherlands', 'Austria']</t>
         </is>
       </c>
       <c r="I249" t="inlineStr">
@@ -13439,7 +13439,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
@@ -13493,7 +13493,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Austria', 'France']</t>
+          <t>['Austria', 'Netherlands', 'France']</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -13535,7 +13535,7 @@
       <c r="G252" t="inlineStr"/>
       <c r="H252" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium', 'Ukraine']</t>
+          <t>['Ukraine', 'Romania', 'Belgium']</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
@@ -13589,7 +13589,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Belgium', 'Ukraine']</t>
+          <t>['Ukraine', 'Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -13643,7 +13643,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium', 'Slovakia']</t>
+          <t>['Romania', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="I254" t="inlineStr">
@@ -13685,7 +13685,7 @@
       <c r="G255" t="inlineStr"/>
       <c r="H255" t="inlineStr">
         <is>
-          <t>['Turkey', 'Czech Republic', 'Portugal']</t>
+          <t>['Czech Republic', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -13739,7 +13739,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>['Turkey', 'Georgia', 'Portugal']</t>
+          <t>['Turkey', 'Portugal', 'Georgia']</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -13793,7 +13793,7 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>['Turkey', 'Georgia', 'Portugal']</t>
+          <t>['Turkey', 'Portugal', 'Georgia']</t>
         </is>
       </c>
       <c r="I257" t="inlineStr">
@@ -13847,7 +13847,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>['Turkey', 'Georgia', 'Portugal']</t>
+          <t>['Turkey', 'Portugal', 'Georgia']</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>['Turkey', 'Georgia', 'Portugal']</t>
+          <t>['Turkey', 'Portugal', 'Georgia']</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
@@ -13955,7 +13955,7 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>['Turkey', 'Georgia', 'Portugal']</t>
+          <t>['Turkey', 'Portugal', 'Georgia']</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">

</xml_diff>